<commit_message>
list splitting to get chains
the list splitting approach is fully implemented, first parts of the analysis
</commit_message>
<xml_diff>
--- a/chain split/splitting_validation.xlsx
+++ b/chain split/splitting_validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P.A. Ruben\Desktop\thesis SEC\1 - SE data\gis.SE.thesis\chain split\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC05EF9B-3823-4FA4-8600-A7626AAF7F5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967F087E-6B8D-4241-AA50-70D58A70B820}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CC4A1E23-83C7-4092-876D-06581A4F3240}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="83">
   <si>
     <t>answer_id</t>
   </si>
@@ -137,13 +137,175 @@
   </si>
   <si>
     <t>need for different dbs/schemas</t>
+  </si>
+  <si>
+    <t>displaying layers</t>
+  </si>
+  <si>
+    <t>pixels and polygon intersection</t>
+  </si>
+  <si>
+    <t>software speed</t>
+  </si>
+  <si>
+    <t>software bug slope computing</t>
+  </si>
+  <si>
+    <t>unclear question on moving points</t>
+  </si>
+  <si>
+    <t>cumulative, on valide polygons</t>
+  </si>
+  <si>
+    <t>discussion on software</t>
+  </si>
+  <si>
+    <t>duplicate</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>admin rights</t>
+  </si>
+  <si>
+    <t>library versions saga</t>
+  </si>
+  <si>
+    <t>uploading data</t>
+  </si>
+  <si>
+    <t>gdal data export</t>
+  </si>
+  <si>
+    <t>tool for arcpy</t>
+  </si>
+  <si>
+    <t>generating points on line</t>
+  </si>
+  <si>
+    <t>arcgis wfs compliance</t>
+  </si>
+  <si>
+    <t>clip raster speed</t>
+  </si>
+  <si>
+    <t>debugging conversation python</t>
+  </si>
+  <si>
+    <t>gdal debug conversation</t>
+  </si>
+  <si>
+    <t>https://chat.stackexchange.com/rooms/76610/discussion-on-answer-by-rodrigo-how-to-create-a-grid-of-10degx10deg-polygons-for</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>2 person debug conv</t>
+  </si>
+  <si>
+    <t>3 person discussion</t>
+  </si>
+  <si>
+    <t>mostly 2 person conv</t>
+  </si>
+  <si>
+    <t>file format conv</t>
+  </si>
+  <si>
+    <t>2 person debug conv, aborted</t>
+  </si>
+  <si>
+    <t>debug conv + 2 comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debug conv </t>
+  </si>
+  <si>
+    <t>development of plugin</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>one message missed</t>
+  </si>
+  <si>
+    <t>messed up</t>
+  </si>
+  <si>
+    <t>python environment</t>
+  </si>
+  <si>
+    <t>cumulative</t>
+  </si>
+  <si>
+    <t>messages in between</t>
+  </si>
+  <si>
+    <t>cumulative cos + conversation</t>
+  </si>
+  <si>
+    <t>several convs</t>
+  </si>
+  <si>
+    <t>two times one message</t>
+  </si>
+  <si>
+    <t>one missed, one added</t>
+  </si>
+  <si>
+    <t>wrongly added</t>
+  </si>
+  <si>
+    <t>missed</t>
+  </si>
+  <si>
+    <t>one chain too much</t>
+  </si>
+  <si>
+    <t>affected chains</t>
+  </si>
+  <si>
+    <t>extreme cumulative</t>
+  </si>
+  <si>
+    <t>qgis tools</t>
+  </si>
+  <si>
+    <t>software in R, limit cumulative</t>
+  </si>
+  <si>
+    <t>bug of qgis</t>
+  </si>
+  <si>
+    <t>bug in qgis</t>
+  </si>
+  <si>
+    <t>settings in esri</t>
+  </si>
+  <si>
+    <t>bug qgis psql</t>
+  </si>
+  <si>
+    <t>cumulative, json</t>
+  </si>
+  <si>
+    <t>debug discussion</t>
+  </si>
+  <si>
+    <t>ge engine</t>
+  </si>
+  <si>
+    <t>psql esri database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,8 +313,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +359,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -192,21 +380,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -223,14 +486,107 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>120590</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>263777</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>142295</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806B604D-98FC-4EF2-9215-E68E469B2B91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8441630" y="6042660"/>
+          <a:ext cx="4410387" cy="2512115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>23867</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>334061</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA53E41C-08D1-4BFC-BF66-5FBFC2182843}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10021307" y="7307580"/>
+          <a:ext cx="3967794" cy="2148840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>309464</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>408524</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>181651</xdr:rowOff>
     </xdr:to>
@@ -255,7 +611,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6370320" y="548640"/>
+          <a:off x="8298180" y="548640"/>
           <a:ext cx="3959444" cy="1461811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -267,14 +623,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>88536</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>187596</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>164963</xdr:rowOff>
     </xdr:to>
@@ -299,7 +655,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6408420" y="3147061"/>
+          <a:off x="8336280" y="3147061"/>
           <a:ext cx="5529216" cy="309742"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -311,14 +667,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>10504</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>109564</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>44768</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>143828</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>178472</xdr:rowOff>
     </xdr:to>
@@ -343,7 +699,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6373204" y="3497580"/>
+          <a:off x="8301064" y="3497580"/>
           <a:ext cx="4911064" cy="3081692"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -358,10 +714,21 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{25DC4784-983F-4D45-99B1-8B4B3139FE9B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="3">
-    <queryTableFields count="2">
+  <queryTableRefresh nextId="14" unboundColumnsRight="11">
+    <queryTableFields count="13">
       <queryTableField id="1" name="answer_id" tableColumnId="1"/>
       <queryTableField id="2" name="count" tableColumnId="2"/>
+      <queryTableField id="3" dataBound="0" tableColumnId="3"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
+      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="8"/>
+      <queryTableField id="12" dataBound="0" tableColumnId="12"/>
+      <queryTableField id="11" dataBound="0" tableColumnId="11"/>
+      <queryTableField id="13" dataBound="0" tableColumnId="13"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="9"/>
+      <queryTableField id="10" dataBound="0" tableColumnId="10"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -379,11 +746,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0718E2F6-1B4F-4489-92E7-53360875E5A8}" name="validation_as" displayName="validation_as" ref="A1:B46" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B46" xr:uid="{BEB34D2F-F4FE-4823-86A2-ECC48ADE6062}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0718E2F6-1B4F-4489-92E7-53360875E5A8}" name="validation_as" displayName="validation_as" ref="A1:M46" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:M46" xr:uid="{BEB34D2F-F4FE-4823-86A2-ECC48ADE6062}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{21EAB19E-8109-472D-B587-B2263CB6B6AD}" uniqueName="1" name="answer_id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{7DC8E536-6AB7-4A1C-9031-9FDD7EF3B1DC}" uniqueName="2" name="count" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{A6B64DEF-C01C-45CC-817F-D14ED9C982B0}" uniqueName="3" name="validation" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{A2B2DA57-187A-46B8-A585-44C42425D8F0}" uniqueName="4" name="uncertainty" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{86FA2592-2C6F-4984-B05F-BFEB31D21968}" uniqueName="5" name="comments" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{26B97E48-182F-4764-9712-FA8FF0CD3BAA}" uniqueName="6" name="chat" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{F8BD220E-19CB-4814-9598-543B3F588EB5}" uniqueName="7" name="closed" queryTableFieldId="7"/>
+    <tableColumn id="8" xr3:uid="{A65260C3-1C3F-4D82-B86D-826C318247E3}" uniqueName="8" name="offensive/defensive" queryTableFieldId="8"/>
+    <tableColumn id="12" xr3:uid="{74B69DC9-1C3D-4B82-A9BF-97F05306A705}" uniqueName="12" name="wrongly added" queryTableFieldId="12" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{C2242ADB-4F21-4216-B58D-44ABABB4DC2B}" uniqueName="11" name="missed" queryTableFieldId="11" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{0E3752B8-D44A-4E65-9066-24A3803A5C65}" uniqueName="13" name="affected chains" queryTableFieldId="13" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{A6430854-98D0-45F6-B04C-A8F3472ACEF4}" uniqueName="9" name="Column1" queryTableFieldId="9"/>
+    <tableColumn id="10" xr3:uid="{B9535FB3-DFC0-431A-BA74-24455A935A72}" uniqueName="10" name="Column2" queryTableFieldId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -697,325 +1075,1152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98DC582-264E-43E8-B386-E128CC33BB16}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>230749</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102122</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7650</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>280958</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>318205</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>199685</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>312501</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>245492</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>86185</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>250432</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>244296</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>306981</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5787</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>34387</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>52231</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>267985</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>272392</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>284414</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>288655</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>176225</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>220274</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>252544</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>267486</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>307271</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>322956</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>21661</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="7">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>33070</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="7">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>126550</v>
       </c>
       <c r="B29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="7">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>209131</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="7">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2</v>
+      </c>
+      <c r="K30" s="8">
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>274600</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="7">
+        <v>3</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>109969</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="7">
+        <v>3</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="8">
+        <v>3</v>
+      </c>
+      <c r="K32" s="8">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5642</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="7">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>22492</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="7">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="M34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>54792</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="7">
+        <v>3</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="8"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>92227</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="7">
+        <v>3</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="8">
+        <v>1</v>
+      </c>
+      <c r="K36" s="8">
+        <v>1</v>
+      </c>
+      <c r="M36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>191446</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="7">
+        <v>4</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+      <c r="J37" s="8">
+        <v>1</v>
+      </c>
+      <c r="K37" s="8">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>31415</v>
       </c>
       <c r="B38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="7">
+        <v>4</v>
+      </c>
+      <c r="D38" s="3">
+        <v>2</v>
+      </c>
+      <c r="I38" s="3">
+        <v>2</v>
+      </c>
+      <c r="K38" s="8">
+        <v>2</v>
+      </c>
+      <c r="M38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>81176</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="7">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>304598</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="7">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="K40" s="8"/>
+      <c r="M40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1105</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" s="7">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="J41" s="8">
+        <v>2</v>
+      </c>
+      <c r="K41" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>104528</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" s="7">
+        <v>3</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="8"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>83027</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" s="7">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="8"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>104380</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>1</v>
+      </c>
+      <c r="K44" s="8">
+        <v>1</v>
+      </c>
+      <c r="M44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>155448</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" s="7">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1</v>
+      </c>
+      <c r="K45" s="8">
+        <v>1</v>
+      </c>
+      <c r="M45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>273718</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
+      <c r="K46" s="8">
+        <v>1</v>
+      </c>
+      <c r="M46" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D531E6-8361-49EE-A1F6-7D7B63120F81}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,9 +2228,10 @@
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1050,8 +2256,17 @@
       <c r="H1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>346059</v>
       </c>
@@ -1073,8 +2288,11 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>282089</v>
       </c>
@@ -1096,8 +2314,11 @@
       <c r="G3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>304516</v>
       </c>
@@ -1119,8 +2340,11 @@
       <c r="G4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>254232</v>
       </c>
@@ -1142,8 +2366,11 @@
       <c r="G5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>313975</v>
       </c>
@@ -1165,8 +2392,11 @@
       <c r="G6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>230605</v>
       </c>
@@ -1188,8 +2418,11 @@
       <c r="G7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>233785</v>
       </c>
@@ -1211,8 +2444,11 @@
       <c r="G8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>273946</v>
       </c>
@@ -1234,8 +2470,11 @@
       <c r="G9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>253475</v>
       </c>
@@ -1257,8 +2496,11 @@
       <c r="G10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>270327</v>
       </c>
@@ -1280,8 +2522,11 @@
       <c r="G11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>277603</v>
       </c>
@@ -1303,8 +2548,11 @@
       <c r="G12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>284652</v>
       </c>
@@ -1326,8 +2574,11 @@
       <c r="G13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>291751</v>
       </c>
@@ -1349,8 +2600,11 @@
       <c r="G14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>304139</v>
       </c>
@@ -1375,8 +2629,11 @@
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>314664</v>
       </c>
@@ -1398,8 +2655,11 @@
       <c r="G16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" s="9"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>332587</v>
       </c>
@@ -1421,8 +2681,15 @@
       <c r="G17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" s="9">
+        <v>1</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>223498</v>
       </c>
@@ -1444,8 +2711,11 @@
       <c r="G18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>224668</v>
       </c>
@@ -1467,8 +2737,11 @@
       <c r="G19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>234630</v>
       </c>
@@ -1490,300 +2763,809 @@
       <c r="G20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>242337</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>258651</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>292368</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>293799</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>306342</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>317620</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6037</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C27" s="3">
+        <v>8</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="9">
+        <v>6</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>32119</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="9">
+        <v>2</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>36795</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C29" s="3">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="9">
+        <v>4</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>310347</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="9">
+        <v>1</v>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>137025</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>137025</v>
       </c>
-      <c r="B32">
-        <v>2</v>
+      <c r="B32" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>144077</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>165950</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C34" s="3">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>18814</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C35" s="3">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="9">
+        <v>1</v>
+      </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>57338</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="3">
+        <v>3</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>64383</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="10">
+        <v>1</v>
+      </c>
+      <c r="K37" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>94469</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="10">
+        <v>3</v>
+      </c>
+      <c r="K38" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>126380</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C39" s="3">
+        <v>3</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="9"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>182670</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C40" s="3">
+        <v>3</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>182670</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="C41" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I41" s="9"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>211000</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C42" s="3">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="9"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>300860</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="9"/>
+      <c r="J43" s="10">
+        <v>3</v>
+      </c>
+      <c r="K43" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>57651</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="10">
+        <v>1</v>
+      </c>
+      <c r="K44" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>216871</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C45" s="3">
+        <v>2</v>
+      </c>
+      <c r="D45" s="4">
+        <v>2</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="9"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>256849</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C46" s="3">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>93159</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C47" s="3">
+        <v>2</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>172504</v>
       </c>
       <c r="B48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="3">
+        <v>2</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="9"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>227384</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="3">
+        <v>3</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="9"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>263629</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
+      <c r="C50" s="3">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="9"/>
+      <c r="J50" s="10">
+        <v>1</v>
+      </c>
+      <c r="K50" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>